<commit_message>
removing some sensitive info
</commit_message>
<xml_diff>
--- a/data/ivsc_4cmtct_shedct_param.xlsx
+++ b/data/ivsc_4cmtct_shedct_param.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/GitHub/IMA_TumorModeling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astein/Github/TumorModelingCode/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="460" windowWidth="24700" windowHeight="16840" tabRatio="500"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="24700" windowHeight="14960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="146">
   <si>
     <t>Parameter</t>
   </si>
@@ -190,15 +190,9 @@
     <t>From PopPK - exp(logV1)</t>
   </si>
   <si>
-    <t>Detail</t>
-  </si>
-  <si>
     <t>From PopPK - exp(logV2)</t>
   </si>
   <si>
-    <t>This number is really questionable.  Probably think a bit more</t>
-  </si>
-  <si>
     <t>Same as VD1</t>
   </si>
   <si>
@@ -247,9 +241,6 @@
     <t>From TMDD ~ exp(log(Kd))</t>
   </si>
   <si>
-    <t>From Table 4-1 of IB v2 (p17), converted to days</t>
-  </si>
-  <si>
     <t>Same as koff1</t>
   </si>
   <si>
@@ -277,9 +268,6 @@
     <t>Same as keD1</t>
   </si>
   <si>
-    <t>From KarthikSubra Slidedeck, slide 16 (log(2)/t1/2 h)*24</t>
-  </si>
-  <si>
     <t>TMDD-Shedding</t>
   </si>
   <si>
@@ -443,12 +431,6 @@
   </si>
   <si>
     <t>From xxx</t>
-  </si>
-  <si>
-    <t>Work/001_Karthik_Varun/POPPK-2_Karthik/NONMEM/run13.lst</t>
-  </si>
-  <si>
-    <t>Work/001_Karthik_Varun/POPPK-2_Karthik/NONMEM/run9.lst</t>
   </si>
   <si>
     <t>Chosen to match the target accumulation.  
@@ -614,15 +596,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -662,7 +635,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1032,76 +1016,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53:F56"/>
+    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="20" style="9" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="20" style="6" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="6" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" style="19" customWidth="1"/>
     <col min="7" max="7" width="9.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="68.83203125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="10" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="10"/>
+    <col min="9" max="9" width="68.83203125" style="11" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>92</v>
+      <c r="B1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="19" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11">
+    </row>
+    <row r="2" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>93</v>
+      <c r="B2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="20">
         <v>0</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1110,27 +1090,27 @@
       <c r="H2" s="4">
         <v>0</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11">
+    <row r="3" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>94</v>
+      <c r="B3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="20">
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1139,57 +1119,57 @@
       <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="11">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>95</v>
+      <c r="B4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="6">
+        <v>49</v>
+      </c>
+      <c r="F4" s="19">
         <f>EXP(-4.552)*24</f>
         <v>0.25310618628986775</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="11">
-        <v>4</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>104</v>
+        <v>68</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="20">
         <f>CL/Vc</f>
         <v>7.7077322733120998E-2</v>
       </c>
@@ -1197,59 +1177,59 @@
         <v>4</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11">
+        <v>69</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>96</v>
+      <c r="B6" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>92</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="6">
+        <v>52</v>
+      </c>
+      <c r="F6" s="19">
         <f>EXP(-3.771)*24</f>
         <v>0.55269654590709449</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="11">
+        <v>68</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>97</v>
+      <c r="B7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="6">
         <f>EXP(1.189)</f>
         <v>3.2837957691686293</v>
       </c>
@@ -1257,32 +1237,29 @@
         <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="11">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>98</v>
+      <c r="B8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="19">
         <f>EXP(0.6221)</f>
         <v>1.862835892541314</v>
       </c>
@@ -1290,29 +1267,29 @@
         <v>2</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="11">
+        <v>68</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>99</v>
+      <c r="B9" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="20">
         <f>F7</f>
         <v>3.2837957691686293</v>
       </c>
@@ -1320,29 +1297,29 @@
         <v>2</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="11">
+        <v>69</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>100</v>
+      <c r="B10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>96</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="20">
         <f>F7</f>
         <v>3.2837957691686293</v>
       </c>
@@ -1350,29 +1327,29 @@
         <v>2</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11">
+        <v>69</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>101</v>
+      <c r="B11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="20">
         <f>Q/Vc</f>
         <v>0.16831026798205015</v>
       </c>
@@ -1380,29 +1357,29 @@
         <v>4</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11">
+        <v>69</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>107</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="20">
         <f>Q/Vp</f>
         <v>0.29669631561215842</v>
       </c>
@@ -1410,87 +1387,84 @@
         <v>4</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I12" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="19">
+        <v>57</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>12</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F13" s="6">
-        <v>57</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11">
-        <v>12</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="6">
+      <c r="F14" s="19">
         <f>EXP(1.22)</f>
         <v>3.3871877336213347</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11">
+        <v>68</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
         <v>13</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>110</v>
+      <c r="B15" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="19">
         <f>0.00007*3600*24</f>
         <v>6.048</v>
       </c>
@@ -1498,29 +1472,27 @@
         <v>4</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11">
+        <v>70</v>
+      </c>
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
         <v>14</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>110</v>
+      <c r="B16" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="19">
         <f>0.00007*3600*24</f>
         <v>6.048</v>
       </c>
@@ -1528,29 +1500,29 @@
         <v>4</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11">
+        <v>69</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
         <v>15</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>111</v>
+      <c r="B17" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="20">
         <f>F15/F14</f>
         <v>1.7855520495564379</v>
       </c>
@@ -1558,29 +1530,29 @@
         <v>20</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11">
+        <v>69</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8">
         <v>16</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>111</v>
+      <c r="B18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="20">
         <f>F17</f>
         <v>1.7855520495564379</v>
       </c>
@@ -1588,27 +1560,27 @@
         <v>20</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" s="12"/>
-    </row>
-    <row r="19" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11">
+        <v>69</v>
+      </c>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
         <v>17</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>104</v>
+      <c r="B19" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>100</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="19">
         <f>LOG(2)/1.4*24</f>
         <v>5.1605142113825355</v>
       </c>
@@ -1616,32 +1588,27 @@
         <v>4</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11">
+        <v>68</v>
+      </c>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8">
         <v>18</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>104</v>
+      <c r="B20" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="20">
         <f>keD</f>
         <v>7.7077322733120998E-2</v>
       </c>
@@ -1649,29 +1616,29 @@
         <v>4</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11">
+        <v>69</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8">
         <v>19</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>112</v>
+      <c r="B21" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="20">
         <v>0</v>
       </c>
       <c r="G21" s="4" t="s">
@@ -1680,27 +1647,27 @@
       <c r="H21" s="4">
         <v>0</v>
       </c>
-      <c r="I21" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11">
+      <c r="I21" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8">
         <v>20</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>112</v>
+      <c r="B22" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="20">
         <v>0</v>
       </c>
       <c r="G22" s="4" t="s">
@@ -1709,27 +1676,27 @@
       <c r="H22" s="4">
         <v>0</v>
       </c>
-      <c r="I22" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="20" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="11">
+      <c r="I22" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="17" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
         <v>21</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>114</v>
+      <c r="B23" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>110</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="21">
         <v>10</v>
       </c>
       <c r="G23" s="3" t="s">
@@ -1738,30 +1705,27 @@
       <c r="H23" s="3">
         <v>1</v>
       </c>
-      <c r="I23" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="J23" s="20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11">
+      <c r="I23" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
         <v>22</v>
       </c>
-      <c r="B24" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>115</v>
+      <c r="B24" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="19">
         <f>LOG(2)/5.4*24</f>
         <v>1.3379110918399164</v>
       </c>
@@ -1769,29 +1733,29 @@
         <v>4</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11">
+        <v>70</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
         <v>23</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>115</v>
+      <c r="B25" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="20">
         <f>kshed</f>
         <v>1.3379110918399164</v>
       </c>
@@ -1799,61 +1763,58 @@
         <v>4</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11">
+        <v>69</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
         <v>24</v>
       </c>
-      <c r="B26" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>117</v>
+      <c r="B26" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>113</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="21">
         <v>0.5</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I26" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="J26" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11">
+        <v>73</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="8">
         <v>25</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>117</v>
+      <c r="B27" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="20">
         <f>Vtum</f>
         <v>0.5</v>
       </c>
@@ -1861,29 +1822,29 @@
         <v>2</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11">
+        <v>69</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
         <v>26</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>117</v>
+      <c r="B28" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="20">
         <f>Vtum</f>
         <v>0.5</v>
       </c>
@@ -1891,29 +1852,29 @@
         <v>2</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11">
+        <v>69</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8">
         <v>27</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>118</v>
+      <c r="B29" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="20">
         <v>0</v>
       </c>
       <c r="G29" s="4" t="s">
@@ -1922,27 +1883,27 @@
       <c r="H29" s="4">
         <v>0</v>
       </c>
-      <c r="I29" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="11">
+      <c r="I29" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="8">
         <v>28</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>119</v>
+      <c r="B30" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="20">
         <v>0</v>
       </c>
       <c r="G30" s="4" t="s">
@@ -1951,27 +1912,27 @@
       <c r="H30" s="4">
         <v>0</v>
       </c>
-      <c r="I30" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="11">
+      <c r="I30" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="8">
         <v>29</v>
       </c>
-      <c r="B31" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>120</v>
+      <c r="B31" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="20">
         <v>0</v>
       </c>
       <c r="G31" s="4" t="s">
@@ -1980,27 +1941,27 @@
       <c r="H31" s="4">
         <v>0</v>
       </c>
-      <c r="I31" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="11">
+      <c r="I31" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="8">
         <v>30</v>
       </c>
-      <c r="B32" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>121</v>
+      <c r="B32" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="20">
         <v>0</v>
       </c>
       <c r="G32" s="4" t="s">
@@ -2009,27 +1970,27 @@
       <c r="H32" s="4">
         <v>0</v>
       </c>
-      <c r="I32" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="11">
+      <c r="I32" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="8">
         <v>31</v>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>122</v>
+      <c r="B33" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="20">
         <v>0</v>
       </c>
       <c r="G33" s="4" t="s">
@@ -2038,85 +1999,85 @@
       <c r="H33" s="4">
         <v>0</v>
       </c>
-      <c r="I33" s="12" t="s">
-        <v>69</v>
+      <c r="I33" s="9" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="11">
+      <c r="A34" s="8">
         <v>32</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D34" s="9" t="s">
+      <c r="B34" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F34" s="6">
+      <c r="F34" s="19">
         <v>0.3</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I34" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="8">
+        <v>33</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="11">
-        <v>33</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F35" s="6">
+      <c r="F35" s="19">
         <v>0.4</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I35" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11">
+        <v>73</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="8">
         <v>34</v>
       </c>
-      <c r="B36" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>123</v>
+      <c r="B36" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="20">
         <f>k12D*Vtum/Vc</f>
         <v>2.5627395826851602E-2</v>
       </c>
@@ -2124,29 +2085,29 @@
         <v>4</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I36" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="11">
+        <v>69</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="8">
         <v>35</v>
       </c>
-      <c r="B37" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>123</v>
+      <c r="B37" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="20">
         <f>k13D*2</f>
         <v>5.1254791653703204E-2</v>
       </c>
@@ -2154,29 +2115,29 @@
         <v>4</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I37" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="11">
+        <v>69</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="8">
         <v>36</v>
       </c>
-      <c r="B38" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>123</v>
+      <c r="B38" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="20">
         <f>k13D</f>
         <v>2.5627395826851602E-2</v>
       </c>
@@ -2184,29 +2145,29 @@
         <v>4</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I38" s="12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="11">
+        <v>69</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="8">
         <v>37</v>
       </c>
-      <c r="B39" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>124</v>
+      <c r="B39" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>120</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="20">
         <f>k13D/ABCdrug*Vc/Vtum</f>
         <v>0.56103422660683377</v>
       </c>
@@ -2214,59 +2175,59 @@
         <v>4</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I39" s="12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="11">
+        <v>69</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="8">
         <v>38</v>
       </c>
-      <c r="B40" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>124</v>
+      <c r="B40" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>120</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="20">
         <f>k13S/ABCsol*VcS/VtumS</f>
         <v>0.84155133991025077</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H40" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="I40" s="13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="11">
+      <c r="H40" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="8">
         <v>39</v>
       </c>
-      <c r="B41" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>124</v>
+      <c r="B41" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>120</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="20">
         <f>k13DS/ABCdrug*VcDS/VtumDS</f>
         <v>0.56103422660683377</v>
       </c>
@@ -2274,29 +2235,29 @@
         <v>4</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I41" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="11">
+        <v>69</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="8">
         <v>40</v>
       </c>
-      <c r="B42" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>112</v>
+      <c r="B42" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>108</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="F42" s="8">
+        <v>130</v>
+      </c>
+      <c r="F42" s="21">
         <v>10</v>
       </c>
       <c r="G42" s="3" t="s">
@@ -2305,25 +2266,25 @@
       <c r="H42" s="3">
         <v>1</v>
       </c>
-      <c r="I42" s="19"/>
-    </row>
-    <row r="43" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="11">
+      <c r="I42" s="16"/>
+    </row>
+    <row r="43" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="8">
         <v>41</v>
       </c>
-      <c r="B43" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>137</v>
+      <c r="B43" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>131</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F43" s="6">
+        <v>132</v>
+      </c>
+      <c r="F43" s="19">
         <f>LOG(2)/5.4*24</f>
         <v>1.3379110918399164</v>
       </c>
@@ -2331,27 +2292,27 @@
         <v>4</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I43" s="16"/>
-    </row>
-    <row r="44" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="11">
+        <v>70</v>
+      </c>
+      <c r="I43" s="13"/>
+    </row>
+    <row r="44" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="8">
         <v>42</v>
       </c>
-      <c r="B44" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>137</v>
+      <c r="B44" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>131</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="F44" s="6">
+        <v>133</v>
+      </c>
+      <c r="F44" s="19">
         <f>LOG(2)/5.4*24</f>
         <v>1.3379110918399164</v>
       </c>
@@ -2359,27 +2320,27 @@
         <v>4</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I44" s="12"/>
-    </row>
-    <row r="45" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="11">
+        <v>69</v>
+      </c>
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="8">
         <v>43</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>121</v>
+      <c r="B45" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F45" s="7">
+        <v>134</v>
+      </c>
+      <c r="F45" s="20">
         <v>0</v>
       </c>
       <c r="G45" s="4" t="s">
@@ -2388,25 +2349,25 @@
       <c r="H45" s="4">
         <v>0</v>
       </c>
-      <c r="I45" s="12"/>
-    </row>
-    <row r="46" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="11">
+      <c r="I45" s="9"/>
+    </row>
+    <row r="46" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="8">
         <v>44</v>
       </c>
-      <c r="B46" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>122</v>
+      <c r="B46" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F46" s="7">
+        <v>135</v>
+      </c>
+      <c r="F46" s="20">
         <v>0</v>
       </c>
       <c r="G46" s="4" t="s">
@@ -2415,25 +2376,25 @@
       <c r="H46" s="4">
         <v>0</v>
       </c>
-      <c r="I46" s="12"/>
-    </row>
-    <row r="47" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="11">
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="8">
         <v>45</v>
       </c>
-      <c r="B47" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>123</v>
+      <c r="B47" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F47" s="7">
+        <v>136</v>
+      </c>
+      <c r="F47" s="20">
         <f>k12D*Vtum/Vc</f>
         <v>2.5627395826851602E-2</v>
       </c>
@@ -2441,110 +2402,110 @@
         <v>4</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I47" s="12"/>
-    </row>
-    <row r="48" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="11">
+        <v>69</v>
+      </c>
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="8">
         <v>46</v>
       </c>
-      <c r="B48" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>124</v>
+      <c r="B48" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>120</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F48" s="7">
+        <v>137</v>
+      </c>
+      <c r="F48" s="20">
         <f>k13D/ABCdrug*Vc/Vtum</f>
         <v>0.56103422660683377</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H48" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="11">
+      <c r="H48" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="8">
         <v>47</v>
       </c>
-      <c r="B49" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>123</v>
+      <c r="B49" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F49" s="7">
+        <v>138</v>
+      </c>
+      <c r="F49" s="20">
         <v>2.5627395826851602E-2</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I49" s="12"/>
-    </row>
-    <row r="50" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="11">
+        <v>69</v>
+      </c>
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8">
         <v>48</v>
       </c>
-      <c r="B50" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>124</v>
+      <c r="B50" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>120</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F50" s="7">
+        <v>139</v>
+      </c>
+      <c r="F50" s="20">
         <v>0.56103422660683377</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I50" s="12"/>
+        <v>69</v>
+      </c>
+      <c r="I50" s="9"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E51" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F51" s="6">
+        <v>140</v>
+      </c>
+      <c r="F51" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E52" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F52" s="6">
+        <v>141</v>
+      </c>
+      <c r="F52" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E53" s="22" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F53" s="22">
         <v>3.2837957690000001</v>
@@ -2552,7 +2513,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E54" s="22" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F54" s="22">
         <v>0.5</v>
@@ -2560,7 +2521,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E55" s="22" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F55" s="22">
         <v>3.2837957690000001</v>
@@ -2568,7 +2529,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E56" s="22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F56" s="22">
         <v>0.5</v>

</xml_diff>